<commit_message>
major updates to code base - data saving
</commit_message>
<xml_diff>
--- a/Trials.xlsx
+++ b/Trials.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Practice"/>
@@ -43,19 +43,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -91,7 +85,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -105,22 +99,10 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
   </cellXfs>
@@ -427,201 +409,201 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="7">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="1">
         <v>90</v>
       </c>
-      <c r="D2" s="7">
-        <v>8</v>
-      </c>
-      <c r="E2" s="7">
+      <c r="D2" s="1">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="7">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1">
         <v>110</v>
       </c>
-      <c r="D3" s="7">
-        <v>8</v>
-      </c>
-      <c r="E3" s="7">
+      <c r="D3" s="1">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="7">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="1">
         <v>70</v>
       </c>
-      <c r="D4" s="7">
-        <v>8</v>
-      </c>
-      <c r="E4" s="7">
+      <c r="D4" s="1">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="7">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="1">
         <v>70</v>
       </c>
-      <c r="D5" s="7">
-        <v>8</v>
-      </c>
-      <c r="E5" s="7">
+      <c r="D5" s="1">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="7">
-        <v>5</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="1">
         <v>110</v>
       </c>
-      <c r="D6" s="7">
-        <v>8</v>
-      </c>
-      <c r="E6" s="7">
+      <c r="D6" s="1">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="7">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1">
         <v>90</v>
       </c>
-      <c r="D7" s="7">
-        <v>8</v>
-      </c>
-      <c r="E7" s="7">
+      <c r="D7" s="1">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="7">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1">
         <v>70</v>
       </c>
-      <c r="D8" s="7">
-        <v>8</v>
-      </c>
-      <c r="E8" s="7">
+      <c r="D8" s="1">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="7">
-        <v>8</v>
-      </c>
-      <c r="B9" s="8" t="s">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="1">
         <v>90</v>
       </c>
-      <c r="D9" s="7">
-        <v>8</v>
-      </c>
-      <c r="E9" s="7">
+      <c r="D9" s="1">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="7">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="1">
         <v>110</v>
       </c>
-      <c r="D10" s="7">
-        <v>8</v>
-      </c>
-      <c r="E10" s="7">
+      <c r="D10" s="1">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="7">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="1">
         <v>70</v>
       </c>
-      <c r="D11" s="7">
-        <v>8</v>
-      </c>
-      <c r="E11" s="7">
+      <c r="D11" s="1">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1">
         <v>0</v>
       </c>
     </row>
@@ -641,367 +623,367 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="7">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="1">
         <v>120</v>
       </c>
-      <c r="D2" s="7">
-        <v>8</v>
-      </c>
-      <c r="E2" s="7">
+      <c r="D2" s="1">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="7">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1">
         <v>60</v>
       </c>
-      <c r="D3" s="7">
-        <v>8</v>
-      </c>
-      <c r="E3" s="7">
+      <c r="D3" s="1">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="7">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="1">
         <v>80</v>
       </c>
-      <c r="D4" s="7">
-        <v>8</v>
-      </c>
-      <c r="E4" s="7">
+      <c r="D4" s="1">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="7">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="1">
         <v>100</v>
       </c>
-      <c r="D5" s="7">
-        <v>8</v>
-      </c>
-      <c r="E5" s="7">
+      <c r="D5" s="1">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="7">
-        <v>5</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="1">
         <v>60</v>
       </c>
-      <c r="D6" s="7">
-        <v>8</v>
-      </c>
-      <c r="E6" s="7">
+      <c r="D6" s="1">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="7">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1">
         <v>80</v>
       </c>
-      <c r="D7" s="7">
-        <v>8</v>
-      </c>
-      <c r="E7" s="7">
+      <c r="D7" s="1">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="7">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1">
         <v>120</v>
       </c>
-      <c r="D8" s="7">
-        <v>8</v>
-      </c>
-      <c r="E8" s="7">
+      <c r="D8" s="1">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="7">
-        <v>8</v>
-      </c>
-      <c r="B9" s="8" t="s">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="1">
         <v>100</v>
       </c>
-      <c r="D9" s="7">
-        <v>8</v>
-      </c>
-      <c r="E9" s="7">
+      <c r="D9" s="1">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="7">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="1">
         <v>100</v>
       </c>
-      <c r="D10" s="7">
-        <v>8</v>
-      </c>
-      <c r="E10" s="7">
+      <c r="D10" s="1">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="7">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="1">
         <v>80</v>
       </c>
-      <c r="D11" s="7">
-        <v>8</v>
-      </c>
-      <c r="E11" s="7">
+      <c r="D11" s="1">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="7">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="1">
         <v>60</v>
       </c>
-      <c r="D12" s="7">
-        <v>8</v>
-      </c>
-      <c r="E12" s="7">
+      <c r="D12" s="1">
+        <v>8</v>
+      </c>
+      <c r="E12" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="7">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="1">
         <v>120</v>
       </c>
-      <c r="D13" s="7">
-        <v>8</v>
-      </c>
-      <c r="E13" s="7">
+      <c r="D13" s="1">
+        <v>8</v>
+      </c>
+      <c r="E13" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="7">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="1">
         <v>60</v>
       </c>
-      <c r="D14" s="7">
-        <v>8</v>
-      </c>
-      <c r="E14" s="7">
+      <c r="D14" s="1">
+        <v>8</v>
+      </c>
+      <c r="E14" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="7">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="1">
         <v>100</v>
       </c>
-      <c r="D15" s="7">
-        <v>8</v>
-      </c>
-      <c r="E15" s="7">
+      <c r="D15" s="1">
+        <v>8</v>
+      </c>
+      <c r="E15" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="7">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="1">
         <v>80</v>
       </c>
-      <c r="D16" s="7">
-        <v>8</v>
-      </c>
-      <c r="E16" s="7">
+      <c r="D16" s="1">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="7">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="1">
         <v>120</v>
       </c>
-      <c r="D17" s="7">
-        <v>8</v>
-      </c>
-      <c r="E17" s="7">
+      <c r="D17" s="1">
+        <v>8</v>
+      </c>
+      <c r="E17" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="7">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="1">
         <v>60</v>
       </c>
-      <c r="D18" s="7">
-        <v>8</v>
-      </c>
-      <c r="E18" s="7">
+      <c r="D18" s="1">
+        <v>8</v>
+      </c>
+      <c r="E18" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="7">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="1">
         <v>100</v>
       </c>
-      <c r="D19" s="7">
-        <v>8</v>
-      </c>
-      <c r="E19" s="7">
+      <c r="D19" s="1">
+        <v>8</v>
+      </c>
+      <c r="E19" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
-      <c r="A20" s="7">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="1">
         <v>80</v>
       </c>
-      <c r="D20" s="7">
-        <v>8</v>
-      </c>
-      <c r="E20" s="7">
+      <c r="D20" s="1">
+        <v>8</v>
+      </c>
+      <c r="E20" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
-      <c r="A21" s="7">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="1">
         <v>120</v>
       </c>
-      <c r="D21" s="7">
-        <v>8</v>
-      </c>
-      <c r="E21" s="7">
+      <c r="D21" s="1">
+        <v>8</v>
+      </c>
+      <c r="E21" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1017,711 +999,711 @@
   </sheetPr>
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="15">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="15">
-      <c r="A2" s="7">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="1">
         <v>120</v>
       </c>
-      <c r="D2" s="7">
-        <v>8</v>
-      </c>
-      <c r="E2" s="7">
+      <c r="D2" s="1">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="15">
-      <c r="A3" s="7">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1">
         <v>60</v>
       </c>
-      <c r="D3" s="7">
-        <v>8</v>
-      </c>
-      <c r="E3" s="7">
+      <c r="D3" s="1">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="15">
-      <c r="A4" s="7">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="1">
         <v>80</v>
       </c>
-      <c r="D4" s="7">
-        <v>8</v>
-      </c>
-      <c r="E4" s="7">
+      <c r="D4" s="1">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="15">
-      <c r="A5" s="7">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="1">
         <v>100</v>
       </c>
-      <c r="D5" s="7">
-        <v>8</v>
-      </c>
-      <c r="E5" s="7">
+      <c r="D5" s="1">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="15">
-      <c r="A6" s="7">
-        <v>5</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="1">
         <v>60</v>
       </c>
-      <c r="D6" s="7">
-        <v>8</v>
-      </c>
-      <c r="E6" s="7">
+      <c r="D6" s="1">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="15">
-      <c r="A7" s="7">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1">
         <v>80</v>
       </c>
-      <c r="D7" s="7">
-        <v>8</v>
-      </c>
-      <c r="E7" s="7">
+      <c r="D7" s="1">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="15">
-      <c r="A8" s="7">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1">
         <v>120</v>
       </c>
-      <c r="D8" s="7">
-        <v>8</v>
-      </c>
-      <c r="E8" s="7">
+      <c r="D8" s="1">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="15">
-      <c r="A9" s="7">
-        <v>8</v>
-      </c>
-      <c r="B9" s="8" t="s">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="1">
         <v>100</v>
       </c>
-      <c r="D9" s="7">
-        <v>8</v>
-      </c>
-      <c r="E9" s="7">
+      <c r="D9" s="1">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="15">
-      <c r="A10" s="7">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="1">
         <v>100</v>
       </c>
-      <c r="D10" s="7">
-        <v>8</v>
-      </c>
-      <c r="E10" s="7">
+      <c r="D10" s="1">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="15">
-      <c r="A11" s="7">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="1">
         <v>80</v>
       </c>
-      <c r="D11" s="7">
-        <v>8</v>
-      </c>
-      <c r="E11" s="7">
+      <c r="D11" s="1">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="15">
-      <c r="A12" s="7">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="1">
         <v>60</v>
       </c>
-      <c r="D12" s="7">
-        <v>8</v>
-      </c>
-      <c r="E12" s="7">
+      <c r="D12" s="1">
+        <v>8</v>
+      </c>
+      <c r="E12" s="1">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="15">
-      <c r="A13" s="7">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="1">
         <v>120</v>
       </c>
-      <c r="D13" s="7">
-        <v>8</v>
-      </c>
-      <c r="E13" s="7">
+      <c r="D13" s="1">
+        <v>8</v>
+      </c>
+      <c r="E13" s="1">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="15">
-      <c r="A14" s="7">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="1">
         <v>60</v>
       </c>
-      <c r="D14" s="7">
-        <v>8</v>
-      </c>
-      <c r="E14" s="7">
+      <c r="D14" s="1">
+        <v>8</v>
+      </c>
+      <c r="E14" s="1">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="15">
-      <c r="A15" s="7">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="1">
         <v>100</v>
       </c>
-      <c r="D15" s="7">
-        <v>8</v>
-      </c>
-      <c r="E15" s="7">
+      <c r="D15" s="1">
+        <v>8</v>
+      </c>
+      <c r="E15" s="1">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="15">
-      <c r="A16" s="7">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="1">
         <v>80</v>
       </c>
-      <c r="D16" s="7">
-        <v>8</v>
-      </c>
-      <c r="E16" s="7">
+      <c r="D16" s="1">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="15">
-      <c r="A17" s="7">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="1">
         <v>120</v>
       </c>
-      <c r="D17" s="7">
-        <v>8</v>
-      </c>
-      <c r="E17" s="7">
+      <c r="D17" s="1">
+        <v>8</v>
+      </c>
+      <c r="E17" s="1">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="15">
-      <c r="A18" s="7">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="1">
         <v>60</v>
       </c>
-      <c r="D18" s="7">
-        <v>8</v>
-      </c>
-      <c r="E18" s="7">
+      <c r="D18" s="1">
+        <v>8</v>
+      </c>
+      <c r="E18" s="1">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="15">
-      <c r="A19" s="7">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="1">
         <v>100</v>
       </c>
-      <c r="D19" s="7">
-        <v>8</v>
-      </c>
-      <c r="E19" s="7">
+      <c r="D19" s="1">
+        <v>8</v>
+      </c>
+      <c r="E19" s="1">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="15">
-      <c r="A20" s="7">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="1">
         <v>80</v>
       </c>
-      <c r="D20" s="7">
-        <v>8</v>
-      </c>
-      <c r="E20" s="7">
+      <c r="D20" s="1">
+        <v>8</v>
+      </c>
+      <c r="E20" s="1">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="15">
-      <c r="A21" s="7">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="1">
         <v>120</v>
       </c>
-      <c r="D21" s="7">
-        <v>8</v>
-      </c>
-      <c r="E21" s="7">
+      <c r="D21" s="1">
+        <v>8</v>
+      </c>
+      <c r="E21" s="1">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="15">
-      <c r="A22" s="7">
+      <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="1">
         <v>120</v>
       </c>
-      <c r="D22" s="7">
-        <v>8</v>
-      </c>
-      <c r="E22" s="7">
+      <c r="D22" s="1">
+        <v>8</v>
+      </c>
+      <c r="E22" s="1">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="15">
-      <c r="A23" s="7">
+      <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="1">
         <v>60</v>
       </c>
-      <c r="D23" s="7">
-        <v>8</v>
-      </c>
-      <c r="E23" s="7">
+      <c r="D23" s="1">
+        <v>8</v>
+      </c>
+      <c r="E23" s="1">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="15">
-      <c r="A24" s="7">
+      <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="1">
         <v>80</v>
       </c>
-      <c r="D24" s="7">
-        <v>8</v>
-      </c>
-      <c r="E24" s="7">
+      <c r="D24" s="1">
+        <v>8</v>
+      </c>
+      <c r="E24" s="1">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="15">
-      <c r="A25" s="7">
+      <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="1">
         <v>100</v>
       </c>
-      <c r="D25" s="7">
-        <v>8</v>
-      </c>
-      <c r="E25" s="7">
+      <c r="D25" s="1">
+        <v>8</v>
+      </c>
+      <c r="E25" s="1">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="15">
-      <c r="A26" s="7">
+      <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C26" s="1">
         <v>60</v>
       </c>
-      <c r="D26" s="7">
-        <v>8</v>
-      </c>
-      <c r="E26" s="7">
+      <c r="D26" s="1">
+        <v>8</v>
+      </c>
+      <c r="E26" s="1">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="15">
-      <c r="A27" s="7">
+      <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="1">
         <v>80</v>
       </c>
-      <c r="D27" s="7">
-        <v>8</v>
-      </c>
-      <c r="E27" s="7">
+      <c r="D27" s="1">
+        <v>8</v>
+      </c>
+      <c r="E27" s="1">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="15">
-      <c r="A28" s="7">
+      <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="1">
         <v>120</v>
       </c>
-      <c r="D28" s="7">
-        <v>8</v>
-      </c>
-      <c r="E28" s="7">
+      <c r="D28" s="1">
+        <v>8</v>
+      </c>
+      <c r="E28" s="1">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="15">
-      <c r="A29" s="7">
+      <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C29" s="1">
         <v>100</v>
       </c>
-      <c r="D29" s="7">
-        <v>8</v>
-      </c>
-      <c r="E29" s="7">
+      <c r="D29" s="1">
+        <v>8</v>
+      </c>
+      <c r="E29" s="1">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="15">
-      <c r="A30" s="7">
+      <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C30" s="1">
         <v>100</v>
       </c>
-      <c r="D30" s="7">
-        <v>8</v>
-      </c>
-      <c r="E30" s="7">
+      <c r="D30" s="1">
+        <v>8</v>
+      </c>
+      <c r="E30" s="1">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="15">
-      <c r="A31" s="7">
-        <v>30</v>
-      </c>
-      <c r="B31" s="8" t="s">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C31" s="1">
         <v>80</v>
       </c>
-      <c r="D31" s="7">
-        <v>8</v>
-      </c>
-      <c r="E31" s="7">
+      <c r="D31" s="1">
+        <v>8</v>
+      </c>
+      <c r="E31" s="1">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="15">
-      <c r="A32" s="7">
+      <c r="A32" s="1">
         <v>31</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="1">
         <v>60</v>
       </c>
-      <c r="D32" s="7">
-        <v>8</v>
-      </c>
-      <c r="E32" s="7">
+      <c r="D32" s="1">
+        <v>8</v>
+      </c>
+      <c r="E32" s="1">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="15">
-      <c r="A33" s="7">
+      <c r="A33" s="1">
         <v>32</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C33" s="1">
         <v>120</v>
       </c>
-      <c r="D33" s="7">
-        <v>8</v>
-      </c>
-      <c r="E33" s="7">
+      <c r="D33" s="1">
+        <v>8</v>
+      </c>
+      <c r="E33" s="1">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="15">
-      <c r="A34" s="7">
+      <c r="A34" s="1">
         <v>33</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C34" s="1">
         <v>60</v>
       </c>
-      <c r="D34" s="7">
-        <v>8</v>
-      </c>
-      <c r="E34" s="7">
+      <c r="D34" s="1">
+        <v>8</v>
+      </c>
+      <c r="E34" s="1">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="15">
-      <c r="A35" s="7">
+      <c r="A35" s="1">
         <v>34</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C35" s="1">
         <v>100</v>
       </c>
-      <c r="D35" s="7">
-        <v>8</v>
-      </c>
-      <c r="E35" s="7">
+      <c r="D35" s="1">
+        <v>8</v>
+      </c>
+      <c r="E35" s="1">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="15">
-      <c r="A36" s="7">
+      <c r="A36" s="1">
         <v>35</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C36" s="1">
         <v>80</v>
       </c>
-      <c r="D36" s="7">
-        <v>8</v>
-      </c>
-      <c r="E36" s="7">
+      <c r="D36" s="1">
+        <v>8</v>
+      </c>
+      <c r="E36" s="1">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="15">
-      <c r="A37" s="7">
+      <c r="A37" s="1">
         <v>36</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C37" s="1">
         <v>120</v>
       </c>
-      <c r="D37" s="7">
-        <v>8</v>
-      </c>
-      <c r="E37" s="7">
+      <c r="D37" s="1">
+        <v>8</v>
+      </c>
+      <c r="E37" s="1">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="15">
-      <c r="A38" s="7">
+      <c r="A38" s="1">
         <v>37</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="1">
         <v>60</v>
       </c>
-      <c r="D38" s="7">
-        <v>8</v>
-      </c>
-      <c r="E38" s="7">
+      <c r="D38" s="1">
+        <v>8</v>
+      </c>
+      <c r="E38" s="1">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="15">
-      <c r="A39" s="7">
+      <c r="A39" s="1">
         <v>38</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C39" s="1">
         <v>100</v>
       </c>
-      <c r="D39" s="7">
-        <v>8</v>
-      </c>
-      <c r="E39" s="7">
+      <c r="D39" s="1">
+        <v>8</v>
+      </c>
+      <c r="E39" s="1">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="15">
-      <c r="A40" s="7">
+      <c r="A40" s="1">
         <v>39</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C40" s="1">
         <v>80</v>
       </c>
-      <c r="D40" s="7">
-        <v>8</v>
-      </c>
-      <c r="E40" s="7">
+      <c r="D40" s="1">
+        <v>8</v>
+      </c>
+      <c r="E40" s="1">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="15">
-      <c r="A41" s="7">
+      <c r="A41" s="1">
         <v>40</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B41" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C41" s="1">
         <v>120</v>
       </c>
-      <c r="D41" s="7">
-        <v>8</v>
-      </c>
-      <c r="E41" s="7">
+      <c r="D41" s="1">
+        <v>8</v>
+      </c>
+      <c r="E41" s="1">
         <v>30</v>
       </c>
     </row>
@@ -1741,367 +1723,367 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="7">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="1">
         <v>120</v>
       </c>
-      <c r="D2" s="7">
-        <v>8</v>
-      </c>
-      <c r="E2" s="7">
+      <c r="D2" s="1">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="7">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1">
         <v>60</v>
       </c>
-      <c r="D3" s="7">
-        <v>8</v>
-      </c>
-      <c r="E3" s="7">
+      <c r="D3" s="1">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="7">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="1">
         <v>80</v>
       </c>
-      <c r="D4" s="7">
-        <v>8</v>
-      </c>
-      <c r="E4" s="7">
+      <c r="D4" s="1">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="7">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="1">
         <v>100</v>
       </c>
-      <c r="D5" s="7">
-        <v>8</v>
-      </c>
-      <c r="E5" s="7">
+      <c r="D5" s="1">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="7">
-        <v>5</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="1">
         <v>60</v>
       </c>
-      <c r="D6" s="7">
-        <v>8</v>
-      </c>
-      <c r="E6" s="7">
+      <c r="D6" s="1">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="7">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1">
         <v>80</v>
       </c>
-      <c r="D7" s="7">
-        <v>8</v>
-      </c>
-      <c r="E7" s="7">
+      <c r="D7" s="1">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="7">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1">
         <v>120</v>
       </c>
-      <c r="D8" s="7">
-        <v>8</v>
-      </c>
-      <c r="E8" s="7">
+      <c r="D8" s="1">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="7">
-        <v>8</v>
-      </c>
-      <c r="B9" s="8" t="s">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="1">
         <v>100</v>
       </c>
-      <c r="D9" s="7">
-        <v>8</v>
-      </c>
-      <c r="E9" s="7">
+      <c r="D9" s="1">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="7">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="1">
         <v>100</v>
       </c>
-      <c r="D10" s="7">
-        <v>8</v>
-      </c>
-      <c r="E10" s="7">
+      <c r="D10" s="1">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="7">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="1">
         <v>80</v>
       </c>
-      <c r="D11" s="7">
-        <v>8</v>
-      </c>
-      <c r="E11" s="7">
+      <c r="D11" s="1">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="7">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="1">
         <v>60</v>
       </c>
-      <c r="D12" s="7">
-        <v>8</v>
-      </c>
-      <c r="E12" s="7">
+      <c r="D12" s="1">
+        <v>8</v>
+      </c>
+      <c r="E12" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="7">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="1">
         <v>120</v>
       </c>
-      <c r="D13" s="7">
-        <v>8</v>
-      </c>
-      <c r="E13" s="7">
+      <c r="D13" s="1">
+        <v>8</v>
+      </c>
+      <c r="E13" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="7">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="1">
         <v>60</v>
       </c>
-      <c r="D14" s="7">
-        <v>8</v>
-      </c>
-      <c r="E14" s="7">
+      <c r="D14" s="1">
+        <v>8</v>
+      </c>
+      <c r="E14" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="7">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="1">
         <v>100</v>
       </c>
-      <c r="D15" s="7">
-        <v>8</v>
-      </c>
-      <c r="E15" s="7">
+      <c r="D15" s="1">
+        <v>8</v>
+      </c>
+      <c r="E15" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="7">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="1">
         <v>80</v>
       </c>
-      <c r="D16" s="7">
-        <v>8</v>
-      </c>
-      <c r="E16" s="7">
+      <c r="D16" s="1">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="7">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="1">
         <v>120</v>
       </c>
-      <c r="D17" s="7">
-        <v>8</v>
-      </c>
-      <c r="E17" s="7">
+      <c r="D17" s="1">
+        <v>8</v>
+      </c>
+      <c r="E17" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="7">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="1">
         <v>60</v>
       </c>
-      <c r="D18" s="7">
-        <v>8</v>
-      </c>
-      <c r="E18" s="7">
+      <c r="D18" s="1">
+        <v>8</v>
+      </c>
+      <c r="E18" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="7">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="1">
         <v>100</v>
       </c>
-      <c r="D19" s="7">
-        <v>8</v>
-      </c>
-      <c r="E19" s="7">
+      <c r="D19" s="1">
+        <v>8</v>
+      </c>
+      <c r="E19" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
-      <c r="A20" s="7">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="1">
         <v>80</v>
       </c>
-      <c r="D20" s="7">
-        <v>8</v>
-      </c>
-      <c r="E20" s="7">
+      <c r="D20" s="1">
+        <v>8</v>
+      </c>
+      <c r="E20" s="1">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
-      <c r="A21" s="7">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="1">
         <v>120</v>
       </c>
-      <c r="D21" s="7">
-        <v>8</v>
-      </c>
-      <c r="E21" s="7">
+      <c r="D21" s="1">
+        <v>8</v>
+      </c>
+      <c r="E21" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2121,8 +2103,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -2173,13 +2155,13 @@
         <f>RAND()</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1">

</xml_diff>